<commit_message>
fix cffs_generator_old and add time analyses
</commit_message>
<xml_diff>
--- a/time_calculator_tables/cff_test_results.xlsx
+++ b/time_calculator_tables/cff_test_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +468,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2804820537567139</v>
+        <v>0.3406929969787598</v>
       </c>
     </row>
     <row r="3">
@@ -484,7 +484,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2612960338592529</v>
+        <v>0.2575700283050537</v>
       </c>
     </row>
     <row r="4">
@@ -500,7 +500,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0.03200793266296387</v>
+        <v>0.009903192520141602</v>
       </c>
     </row>
     <row r="5">
@@ -516,7 +516,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0024261474609375</v>
+        <v>0.0007691383361816406</v>
       </c>
     </row>
     <row r="6">
@@ -532,7 +532,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1341731548309326</v>
+        <v>0.07412600517272949</v>
       </c>
     </row>
     <row r="7">
@@ -548,7 +548,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1156938076019287</v>
+        <v>0.03745579719543457</v>
       </c>
     </row>
     <row r="8">
@@ -558,13 +558,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" t="n">
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2356278896331787</v>
+        <v>0.009923219680786133</v>
       </c>
     </row>
     <row r="9">
@@ -574,13 +574,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C9" t="n">
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>1.069493055343628</v>
+        <v>4.33816385269165</v>
       </c>
     </row>
     <row r="10">
@@ -590,13 +590,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C10" t="n">
         <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>0.7101449966430664</v>
+        <v>2.093926191329956</v>
       </c>
     </row>
     <row r="11">
@@ -606,13 +606,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" t="n">
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0.009562015533447266</v>
+        <v>0.00992894172668457</v>
       </c>
     </row>
     <row r="12">
@@ -622,13 +622,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C12" t="n">
         <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>7.259140729904175</v>
+        <v>64.24477481842041</v>
       </c>
     </row>
     <row r="13">
@@ -638,13 +638,109 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C13" t="n">
         <v>2</v>
       </c>
       <c r="D13" t="n">
-        <v>6.566590070724487</v>
+        <v>33.1779158115387</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Initial CFF</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.2419688701629639</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Grow CFF</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>9</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.7095961570739746</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Direct CFF</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>9</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.2056238651275635</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Initial CFF</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.003067970275878906</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Grow CFF</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>9</v>
+      </c>
+      <c r="C18" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" t="n">
+        <v>3.822492122650146</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Direct CFF</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>9</v>
+      </c>
+      <c r="C19" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1.816632032394409</v>
       </c>
     </row>
   </sheetData>

</xml_diff>